<commit_message>
add working model sans random vars
</commit_message>
<xml_diff>
--- a/food_and_packaging_emissions.xlsx
+++ b/food_and_packaging_emissions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samclymer/Desktop/classes/BEE4750/final_project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samclymer/Desktop/classes/BEE4750/MealEmissions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AFF0CCB3-22D7-0F4B-968F-B3EAD2650080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A71DF819-378A-514F-9EC3-5A9F3DE5B089}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{B6F5DD20-2121-564C-A4CF-C890E70B2901}"/>
   </bookViews>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD7A3CE-D4BA-5742-9FD3-806AAE0EC64E}">
   <dimension ref="A1:C68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>